<commit_message>
LF Denoising results (noisy)
</commit_message>
<xml_diff>
--- a/Denoise_results.xlsx
+++ b/Denoise_results.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="30">
   <si>
     <t>Bikes</t>
   </si>
@@ -61,6 +61,54 @@
   </si>
   <si>
     <t>EPFL</t>
+  </si>
+  <si>
+    <t>Magnets_1</t>
+  </si>
+  <si>
+    <t>Stone_Pillars_Outside</t>
+  </si>
+  <si>
+    <t>Vespa</t>
+  </si>
+  <si>
+    <t>Amethyst</t>
+  </si>
+  <si>
+    <t>Bracelet</t>
+  </si>
+  <si>
+    <t>Chess</t>
+  </si>
+  <si>
+    <t>Eucalyptus Flowers</t>
+  </si>
+  <si>
+    <t>STANFORD</t>
+  </si>
+  <si>
+    <t>Jelly Beens</t>
+  </si>
+  <si>
+    <t>Lego Bulldozer</t>
+  </si>
+  <si>
+    <t>Lego Knights</t>
+  </si>
+  <si>
+    <t>Lego Truck</t>
+  </si>
+  <si>
+    <t>Treasure</t>
+  </si>
+  <si>
+    <t>Average EPFL</t>
+  </si>
+  <si>
+    <t>Average STANFORD</t>
+  </si>
+  <si>
+    <t>Average Overall</t>
   </si>
 </sst>
 </file>
@@ -107,7 +155,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -122,6 +170,8 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -402,10 +452,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -498,6 +548,9 @@
       <c r="B6" s="3" t="s">
         <v>13</v>
       </c>
+      <c r="C6" s="5">
+        <v>26.2822</v>
+      </c>
       <c r="F6" s="5">
         <v>34.997199999999999</v>
       </c>
@@ -509,6 +562,9 @@
       <c r="B7" s="3" t="s">
         <v>13</v>
       </c>
+      <c r="C7" s="5">
+        <v>26.125699999999998</v>
+      </c>
       <c r="F7" s="5">
         <v>34.635599999999997</v>
       </c>
@@ -520,11 +576,217 @@
       <c r="B8" s="3" t="s">
         <v>13</v>
       </c>
+      <c r="C8" s="5">
+        <v>26.448899999999998</v>
+      </c>
       <c r="F8" s="5">
         <v>34.682499999999997</v>
       </c>
     </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="5">
+        <v>25.756900000000002</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="5">
+        <v>26.100300000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" s="5">
+        <v>26.521100000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" s="5">
+        <v>26.736499999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" s="5">
+        <v>25.661300000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" s="5">
+        <v>25.9557</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" s="5">
+        <v>26.973600000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16" s="5">
+        <v>25.677800000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17" s="5">
+        <v>26.433</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>24</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C18" s="5">
+        <v>25.778600000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C19" s="5">
+        <v>26.147600000000001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C20" s="5">
+        <v>26.682500000000001</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A21" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B21" s="7"/>
+      <c r="C21" s="5">
+        <f>AVERAGE(C2:C11)</f>
+        <v>26.207510000000003</v>
+      </c>
+      <c r="D21" s="5" t="e">
+        <f t="shared" ref="D21:F21" si="0">AVERAGE(D2:D11)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E21" s="5" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F21" s="5">
+        <f t="shared" si="0"/>
+        <v>35.331814285714287</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A22" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B22" s="6"/>
+      <c r="C22" s="5">
+        <f>AVERAGE(C12:C20)</f>
+        <v>26.227400000000003</v>
+      </c>
+      <c r="D22" s="5" t="e">
+        <f t="shared" ref="D22:F22" si="1">AVERAGE(D12:D20)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E22" s="5" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F22" s="5" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A23" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B23" s="6"/>
+      <c r="C23" s="5">
+        <f>AVERAGE(C2:C20)</f>
+        <v>26.216931578947364</v>
+      </c>
+      <c r="D23" s="5" t="e">
+        <f t="shared" ref="D23:F23" si="2">AVERAGE(D2:D20)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E23" s="5" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F23" s="5">
+        <f t="shared" si="2"/>
+        <v>35.331814285714287</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A23:B23"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>